<commit_message>
Page 3 SOW: defaultNote support, remove Notes column, scale to 25 install items
- Add defaultNote field to InstallationService/InstallationItem types
- Populate defaultNote for all 82 pricebook installation services
- Pass defaultNote through forms, context, and template creation
- Remove Notes column from PDF Page 3 (Item + Quantity only, more room for names)
- Remove Notes column from EVSE webapp table (not output anywhere)
- EVSE: 4 PDF slots (3 user items + auto EV Parking Signs), webapp warns at limit
- Installation: 25 PDF slots (up from 20), row height 15px, webapp warns at limit
- Add Delete All button with confirmation to Installation Scope form
- Add CLEAR_INSTALLATION_ITEMS reducer action
- Quantities use comma separators in PDF output
- Add Notes column to pricebook Excel export, regenerate CSEV-PriceBook.xlsx

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/CSEV-PriceBook.xlsx
+++ b/data/CSEV-PriceBook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="362">
   <si>
     <t>ID</t>
   </si>
@@ -353,6 +353,9 @@
     <t>Subgroup</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>service-200a-208v</t>
   </si>
   <si>
@@ -368,6 +371,9 @@
     <t>Panels/Switchgear - New Service</t>
   </si>
   <si>
+    <t>Includes Panel + CIAC</t>
+  </si>
+  <si>
     <t>service-400a-208v</t>
   </si>
   <si>
@@ -491,6 +497,9 @@
     <t>Breakers</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>breaker-50a-2p</t>
   </si>
   <si>
@@ -668,6 +677,9 @@
     <t>Install Pad / Vault for Transformer</t>
   </si>
   <si>
+    <t>Includes Pad/Vault</t>
+  </si>
+  <si>
     <t>conduit-40a-pvc-2in</t>
   </si>
   <si>
@@ -780,6 +792,9 @@
   </si>
   <si>
     <t>Install hand hole in grass, 1 per 200'</t>
+  </si>
+  <si>
+    <t>1 per 200'</t>
   </si>
   <si>
     <t>wire-40a</t>
@@ -3101,7 +3116,7 @@
   <sheetPr>
     <tabColor rgb="4CBC88"/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3115,10 +3130,10 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="7" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3140,16 +3155,19 @@
       <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D2" s="3">
         <v>1000</v>
@@ -3158,21 +3176,24 @@
         <v>5000</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D3" s="3">
         <v>3500</v>
@@ -3181,21 +3202,24 @@
         <v>5000</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D4" s="3">
         <v>12000</v>
@@ -3204,21 +3228,24 @@
         <v>5000</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D5" s="3">
         <v>15000</v>
@@ -3227,21 +3254,24 @@
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3">
         <v>17500</v>
@@ -3250,21 +3280,24 @@
         <v>5000</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D7" s="3">
         <v>20000</v>
@@ -3273,21 +3306,24 @@
         <v>5000</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D8" s="3">
         <v>30000</v>
@@ -3296,21 +3332,24 @@
         <v>5000</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D9" s="3">
         <v>50000</v>
@@ -3319,21 +3358,24 @@
         <v>5000</v>
       </c>
       <c r="F9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" t="s">
         <v>116</v>
-      </c>
-      <c r="G9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
       </c>
       <c r="D10" s="3">
         <v>16000</v>
@@ -3342,21 +3384,24 @@
         <v>15000</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D11" s="3">
         <v>23500</v>
@@ -3365,21 +3410,24 @@
         <v>15000</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3">
         <v>25000</v>
@@ -3388,21 +3436,24 @@
         <v>15000</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D13" s="3">
         <v>30000</v>
@@ -3411,21 +3462,24 @@
         <v>15000</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D14" s="3">
         <v>40000</v>
@@ -3434,21 +3488,24 @@
         <v>15000</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D15" s="3">
         <v>55000</v>
@@ -3457,21 +3514,24 @@
         <v>15000</v>
       </c>
       <c r="F15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D16" s="3">
         <v>60000</v>
@@ -3480,21 +3540,24 @@
         <v>15000</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D17" s="3">
         <v>65000</v>
@@ -3503,21 +3566,24 @@
         <v>15000</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D18" s="3">
         <v>50</v>
@@ -3526,21 +3592,24 @@
         <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D19" s="3">
         <v>75</v>
@@ -3549,21 +3618,24 @@
         <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D20" s="3">
         <v>100</v>
@@ -3572,21 +3644,24 @@
         <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D21" s="3">
         <v>100</v>
@@ -3595,21 +3670,24 @@
         <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D22" s="3">
         <v>200</v>
@@ -3618,21 +3696,24 @@
         <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D23" s="3">
         <v>300</v>
@@ -3641,21 +3722,24 @@
         <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D24" s="3">
         <v>400</v>
@@ -3664,21 +3748,24 @@
         <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D25" s="3">
         <v>1000</v>
@@ -3687,21 +3774,24 @@
         <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D26" s="3">
         <v>1250</v>
@@ -3710,21 +3800,24 @@
         <v>200</v>
       </c>
       <c r="F26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B27" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D27" s="3">
         <v>1500</v>
@@ -3733,21 +3826,24 @@
         <v>200</v>
       </c>
       <c r="F27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C28" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D28" s="3">
         <v>2000</v>
@@ -3756,21 +3852,24 @@
         <v>200</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B29" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D29" s="3">
         <v>2500</v>
@@ -3779,21 +3878,24 @@
         <v>200</v>
       </c>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C30" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D30" s="3">
         <v>500</v>
@@ -3802,21 +3904,24 @@
         <v>3500</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D31" s="3">
         <v>1500</v>
@@ -3825,21 +3930,24 @@
         <v>3500</v>
       </c>
       <c r="F31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G31" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D32" s="3">
         <v>2500</v>
@@ -3848,21 +3956,24 @@
         <v>4000</v>
       </c>
       <c r="F32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G32" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D33" s="3">
         <v>3500</v>
@@ -3871,21 +3982,24 @@
         <v>5000</v>
       </c>
       <c r="F33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G33" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C34" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D34" s="3">
         <v>4950</v>
@@ -3894,21 +4008,24 @@
         <v>5000</v>
       </c>
       <c r="F34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G34" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="H34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D35" s="3">
         <v>4500</v>
@@ -3917,21 +4034,24 @@
         <v>2500</v>
       </c>
       <c r="F35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G35" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="H35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C36" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D36" s="3">
         <v>6500</v>
@@ -3940,21 +4060,24 @@
         <v>2500</v>
       </c>
       <c r="F36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G36" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="H36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D37" s="3">
         <v>9000</v>
@@ -3963,21 +4086,24 @@
         <v>12500</v>
       </c>
       <c r="F37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G37" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="H37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D38" s="3">
         <v>3</v>
@@ -3986,21 +4112,24 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G38" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B39" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C39" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D39" s="3">
         <v>4</v>
@@ -4009,21 +4138,24 @@
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B40" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C40" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D40" s="3">
         <v>3</v>
@@ -4032,21 +4164,24 @@
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G40" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" t="s">
         <v>229</v>
-      </c>
-      <c r="C41" t="s">
-        <v>225</v>
       </c>
       <c r="D41" s="3">
         <v>4</v>
@@ -4055,21 +4190,24 @@
         <v>5</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G41" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C42" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D42" s="3">
         <v>3</v>
@@ -4078,21 +4216,24 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G42" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C43" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D43" s="3">
         <v>4</v>
@@ -4101,21 +4242,24 @@
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G43" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H43" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B44" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D44" s="3">
         <v>6</v>
@@ -4124,21 +4268,24 @@
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G44" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B45" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C45" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D45" s="3">
         <v>6</v>
@@ -4147,21 +4294,24 @@
         <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B46" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D46" s="3">
         <v>14</v>
@@ -4170,21 +4320,24 @@
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G46" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H46" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B47" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D47" s="3">
         <v>14</v>
@@ -4193,21 +4346,24 @@
         <v>6</v>
       </c>
       <c r="F47" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G47" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>248</v>
+      </c>
+      <c r="B48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C48" t="s">
         <v>244</v>
-      </c>
-      <c r="B48" t="s">
-        <v>245</v>
-      </c>
-      <c r="C48" t="s">
-        <v>240</v>
       </c>
       <c r="D48" s="3">
         <v>14</v>
@@ -4216,21 +4372,24 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G48" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C49" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D49" s="3">
         <v>16</v>
@@ -4239,21 +4398,24 @@
         <v>7</v>
       </c>
       <c r="F49" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G49" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H49" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B50" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C50" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D50" s="3">
         <v>125</v>
@@ -4262,21 +4424,24 @@
         <v>125</v>
       </c>
       <c r="F50" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="G50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B51" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C51" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D51" s="3">
         <v>100</v>
@@ -4285,21 +4450,24 @@
         <v>50</v>
       </c>
       <c r="F51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G51" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="H51" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C52" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D52" s="3">
         <v>1</v>
@@ -4308,21 +4476,24 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G52" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H52" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C53" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D53" s="3">
         <v>2</v>
@@ -4331,21 +4502,24 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G53" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H53" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B54" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C54" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D54" s="3">
         <v>2</v>
@@ -4354,21 +4528,24 @@
         <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G54" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B55" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C55" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D55" s="3">
         <v>3</v>
@@ -4377,21 +4554,24 @@
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G55" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H55" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B56" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C56" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="D56" s="3">
         <v>7</v>
@@ -4400,21 +4580,24 @@
         <v>3</v>
       </c>
       <c r="F56" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G56" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B57" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C57" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="D57" s="3">
         <v>9</v>
@@ -4423,21 +4606,24 @@
         <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G57" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B58" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C58" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="D58" s="3">
         <v>12</v>
@@ -4446,21 +4632,24 @@
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B59" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C59" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="D59" s="3">
         <v>6</v>
@@ -4469,21 +4658,24 @@
         <v>3</v>
       </c>
       <c r="F59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G59" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B60" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="C60" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="D60" s="3">
         <v>8</v>
@@ -4492,21 +4684,24 @@
         <v>3</v>
       </c>
       <c r="F60" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G60" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H60" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B61" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C61" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D61" s="3">
         <v>100</v>
@@ -4515,21 +4710,24 @@
         <v>200</v>
       </c>
       <c r="F61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G61" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H61" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B62" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C62" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="D62" s="3">
         <v>100</v>
@@ -4538,21 +4736,24 @@
         <v>1250</v>
       </c>
       <c r="F62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G62" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B63" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C63" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D63" s="3">
         <v>100</v>
@@ -4561,21 +4762,24 @@
         <v>100</v>
       </c>
       <c r="F63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H63" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B64" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C64" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="D64" s="3">
         <v>0</v>
@@ -4584,21 +4788,24 @@
         <v>100</v>
       </c>
       <c r="F64" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G64" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B65" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C65" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D65" s="3">
         <v>0</v>
@@ -4607,21 +4814,24 @@
         <v>12.5</v>
       </c>
       <c r="F65" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G65" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="H65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B66" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C66" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="D66" s="3">
         <v>0</v>
@@ -4630,21 +4840,24 @@
         <v>30</v>
       </c>
       <c r="F66" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G66" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="H66" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B67" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C67" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D67" s="3">
         <v>0</v>
@@ -4653,21 +4866,24 @@
         <v>30</v>
       </c>
       <c r="F67" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G67" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="H67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B68" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C68" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D68" s="3">
         <v>0</v>
@@ -4676,21 +4892,24 @@
         <v>50</v>
       </c>
       <c r="F68" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G68" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="H68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B69" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C69" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D69" s="3">
         <v>500</v>
@@ -4699,21 +4918,24 @@
         <v>300</v>
       </c>
       <c r="F69" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G69" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H69" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B70" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C70" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D70" s="3">
         <v>500</v>
@@ -4722,21 +4944,24 @@
         <v>1000</v>
       </c>
       <c r="F70" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G70" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H70" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B71" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C71" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D71" s="3">
         <v>500</v>
@@ -4745,21 +4970,24 @@
         <v>750</v>
       </c>
       <c r="F71" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G71" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B72" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C72" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="D72" s="3">
         <v>150</v>
@@ -4768,21 +4996,24 @@
         <v>150</v>
       </c>
       <c r="F72" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G72" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H72" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="B73" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C73" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D73" s="3">
         <v>100</v>
@@ -4791,21 +5022,24 @@
         <v>900</v>
       </c>
       <c r="F73" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G73" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H73" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B74" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C74" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="D74" s="3">
         <v>100</v>
@@ -4814,21 +5048,24 @@
         <v>900</v>
       </c>
       <c r="F74" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G74" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="B75" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C75" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D75" s="3">
         <v>100</v>
@@ -4837,21 +5074,24 @@
         <v>100</v>
       </c>
       <c r="F75" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G75" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="H75" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B76" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C76" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="D76" s="3">
         <v>1000</v>
@@ -4860,21 +5100,24 @@
         <v>1000</v>
       </c>
       <c r="F76" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="G76" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+      <c r="H76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B77" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="C77" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="D77" s="3">
         <v>1000</v>
@@ -4883,21 +5126,24 @@
         <v>1000</v>
       </c>
       <c r="F77" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="G77" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="H77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B78" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C78" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="D78" s="3">
         <v>2500</v>
@@ -4906,21 +5152,24 @@
         <v>2500</v>
       </c>
       <c r="F78" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="G78" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="H78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="B79" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C79" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="D79" s="3">
         <v>0</v>
@@ -4929,21 +5178,24 @@
         <v>3000</v>
       </c>
       <c r="F79" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="G79" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="H79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B80" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C80" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D80" s="3">
         <v>0</v>
@@ -4952,21 +5204,24 @@
         <v>5500</v>
       </c>
       <c r="F80" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="G80" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="H80" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="B81" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C81" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="D81" s="3">
         <v>0</v>
@@ -4975,21 +5230,24 @@
         <v>300</v>
       </c>
       <c r="F81" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G81" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="H81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="B82" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="C82" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="D82" s="3">
         <v>0</v>
@@ -4998,21 +5256,24 @@
         <v>100</v>
       </c>
       <c r="F82" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G82" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="H82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B83" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="C83" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="D83" s="3">
         <v>0</v>
@@ -5021,10 +5282,13 @@
         <v>50</v>
       </c>
       <c r="F83" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G83" t="s">
-        <v>350</v>
+        <v>355</v>
+      </c>
+      <c r="H83" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>